<commit_message>
Use dataset with *most* things fixed
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11EBC1B-EACB-6144-830A-4C171AB97F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEF82EB-96F8-7F41-ABE4-9FB21B485E14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8ACADFD3-D4EE-4ABF-AACA-8F0EE7039D4B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{8ACADFD3-D4EE-4ABF-AACA-8F0EE7039D4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1774" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1774" uniqueCount="235">
   <si>
     <t>Compound (SMILES)</t>
   </si>
@@ -603,9 +603,6 @@
   </si>
   <si>
     <t>rNaV1.4 T759C</t>
-  </si>
-  <si>
-    <t>IrNaV1.4 1242C</t>
   </si>
   <si>
     <t>rNaV1.4 A1245C</t>
@@ -1222,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FC3777-24FE-4B88-BA57-2E8BD12CE519}">
   <dimension ref="A1:O253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="72" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="72" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1258,16 +1255,16 @@
         <v>179</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>161</v>
@@ -1276,10 +1273,10 @@
         <v>30</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1296,7 +1293,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F2" s="3">
         <v>6.1000000000000004E-3</v>
@@ -1344,7 +1341,7 @@
         <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F3" s="3">
         <v>6.5000000000000002E-2</v>
@@ -1392,7 +1389,7 @@
         <v>46</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F4" s="3">
         <v>0.28000000000000003</v>
@@ -1440,7 +1437,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1488,7 +1485,7 @@
         <v>45</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F6" s="7">
         <v>1.2</v>
@@ -1533,7 +1530,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>177</v>
@@ -1584,7 +1581,7 @@
         <v>188</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F8" s="3">
         <v>1.3</v>
@@ -1680,7 +1677,7 @@
         <v>183</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F10" s="3">
         <v>1.6</v>
@@ -1725,7 +1722,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>177</v>
@@ -1776,7 +1773,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F12" s="3">
         <v>1.9</v>
@@ -1821,7 +1818,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>177</v>
@@ -1920,7 +1917,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F15" s="3">
         <v>2.2999999999999998</v>
@@ -1965,7 +1962,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F16" s="10">
         <v>2.9</v>
@@ -2013,7 +2010,7 @@
         <v>189</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F17" s="3">
         <v>3.1</v>
@@ -2061,7 +2058,7 @@
         <v>184</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F18" s="3">
         <v>3.3</v>
@@ -2157,7 +2154,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F20" s="3">
         <v>4.5</v>
@@ -2253,7 +2250,7 @@
         <v>23</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F22" s="3">
         <v>4.9000000000000004</v>
@@ -2301,7 +2298,7 @@
         <v>25</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F23" s="3">
         <v>5</v>
@@ -2346,7 +2343,7 @@
         <v>55</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F24" s="3">
         <v>5.7</v>
@@ -2394,7 +2391,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F25" s="3">
         <v>6.1</v>
@@ -2442,7 +2439,7 @@
         <v>38</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F26" s="3">
         <v>6.3</v>
@@ -2490,7 +2487,7 @@
         <v>188</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F27" s="3">
         <v>7.2</v>
@@ -2538,7 +2535,7 @@
         <v>47</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F28" s="3">
         <v>7.8</v>
@@ -2586,7 +2583,7 @@
         <v>51</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F29" s="3">
         <v>7.8</v>
@@ -2634,7 +2631,7 @@
         <v>24</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F30" s="3">
         <v>8.1999999999999993</v>
@@ -2682,7 +2679,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F31" s="3">
         <v>8.6999999999999993</v>
@@ -2728,7 +2725,7 @@
         <v>6</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F32" s="7">
         <v>9</v>
@@ -2776,7 +2773,7 @@
         <v>183</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F33" s="3">
         <v>9.1999999999999993</v>
@@ -2824,7 +2821,7 @@
         <v>45</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F34" s="3">
         <v>10</v>
@@ -2872,7 +2869,7 @@
         <v>6</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F35" s="3">
         <v>11</v>
@@ -2917,7 +2914,7 @@
         <v>91</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>177</v>
@@ -2968,7 +2965,7 @@
         <v>38</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F37" s="3">
         <v>13</v>
@@ -3016,7 +3013,7 @@
         <v>185</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F38" s="3">
         <v>14</v>
@@ -3064,7 +3061,7 @@
         <v>6</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F39" s="7">
         <v>14.9</v>
@@ -3112,7 +3109,7 @@
         <v>38</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F40" s="3">
         <v>15</v>
@@ -3160,7 +3157,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F41" s="3">
         <v>17</v>
@@ -3208,7 +3205,7 @@
         <v>37</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F42" s="3">
         <v>17</v>
@@ -3256,7 +3253,7 @@
         <v>6</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F43" s="10">
         <v>17.100000000000001</v>
@@ -3304,7 +3301,7 @@
         <v>20</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F44" s="7">
         <v>18.600000000000001</v>
@@ -3352,7 +3349,7 @@
         <v>20</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F45" s="3">
         <v>19</v>
@@ -3397,7 +3394,7 @@
         <v>91</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>177</v>
@@ -3427,7 +3424,7 @@
       </c>
       <c r="N46" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>ligand_IrNaV1.4.1242C_STX.N21.3</v>
+        <v>ligand_rNaV1.4.1242C_STX.N21.3</v>
       </c>
       <c r="O46" s="2">
         <f t="shared" si="3"/>
@@ -3448,7 +3445,7 @@
         <v>6</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F47" s="3">
         <v>19</v>
@@ -3496,7 +3493,7 @@
         <v>28</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F48" s="3">
         <v>21</v>
@@ -3541,7 +3538,7 @@
         <v>91</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>177</v>
@@ -3592,7 +3589,7 @@
         <v>25</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F50" s="3">
         <v>22</v>
@@ -3640,7 +3637,7 @@
         <v>6</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F51" s="3">
         <v>22</v>
@@ -3688,7 +3685,7 @@
         <v>28</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F52" s="3">
         <v>23</v>
@@ -3736,7 +3733,7 @@
         <v>28</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F53" s="3">
         <v>23</v>
@@ -3784,7 +3781,7 @@
         <v>187</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F54" s="3">
         <v>23</v>
@@ -3832,7 +3829,7 @@
         <v>45</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F55" s="3">
         <v>24</v>
@@ -3880,7 +3877,7 @@
         <v>22</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F56" s="3">
         <v>24</v>
@@ -3928,7 +3925,7 @@
         <v>184</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F57" s="3">
         <v>25</v>
@@ -3976,7 +3973,7 @@
         <v>6</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F58" s="7">
         <v>26</v>
@@ -4024,7 +4021,7 @@
         <v>24</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F59" s="3">
         <v>26</v>
@@ -4072,7 +4069,7 @@
         <v>189</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F60" s="3">
         <v>29</v>
@@ -4120,7 +4117,7 @@
         <v>45</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F61" s="3">
         <v>32</v>
@@ -4168,7 +4165,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F62" s="3">
         <v>34</v>
@@ -4216,7 +4213,7 @@
         <v>6</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F63" s="3">
         <v>35</v>
@@ -4264,7 +4261,7 @@
         <v>6</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F64" s="3">
         <v>35</v>
@@ -4312,7 +4309,7 @@
         <v>41</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F65" s="3">
         <v>36</v>
@@ -4360,7 +4357,7 @@
         <v>45</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F66" s="3">
         <v>38</v>
@@ -4408,7 +4405,7 @@
         <v>45</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F67" s="3">
         <v>38</v>
@@ -4456,7 +4453,7 @@
         <v>45</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F68" s="3">
         <v>38</v>
@@ -4504,7 +4501,7 @@
         <v>23</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F69" s="3">
         <v>38</v>
@@ -4552,7 +4549,7 @@
         <v>37</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F70" s="3">
         <v>39</v>
@@ -4600,7 +4597,7 @@
         <v>41</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F71" s="3">
         <v>41</v>
@@ -4696,7 +4693,7 @@
         <v>37</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F73" s="3">
         <v>43</v>
@@ -4744,7 +4741,7 @@
         <v>22</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F74" s="3">
         <v>44</v>
@@ -4792,7 +4789,7 @@
         <v>6</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F75" s="3">
         <v>46</v>
@@ -4840,7 +4837,7 @@
         <v>186</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F76" s="3">
         <v>48</v>
@@ -4888,7 +4885,7 @@
         <v>6</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F77" s="3">
         <v>54</v>
@@ -4936,7 +4933,7 @@
         <v>45</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F78" s="3">
         <v>56</v>
@@ -4984,7 +4981,7 @@
         <v>23</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F79" s="7">
         <v>63</v>
@@ -5032,7 +5029,7 @@
         <v>45</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F80" s="3">
         <v>66</v>
@@ -5128,7 +5125,7 @@
         <v>183</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F82" s="3">
         <v>77</v>
@@ -5176,7 +5173,7 @@
         <v>6</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F83" s="3">
         <v>78</v>
@@ -5224,7 +5221,7 @@
         <v>41</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F84" s="3">
         <v>78</v>
@@ -5272,7 +5269,7 @@
         <v>23</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F85" s="3">
         <v>80</v>
@@ -5320,7 +5317,7 @@
         <v>184</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F86" s="3">
         <v>80</v>
@@ -5368,7 +5365,7 @@
         <v>6</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F87" s="3">
         <v>83</v>
@@ -5416,7 +5413,7 @@
         <v>6</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F88" s="10">
         <v>83</v>
@@ -5464,7 +5461,7 @@
         <v>22</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F89" s="7">
         <v>84</v>
@@ -5512,7 +5509,7 @@
         <v>6</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F90" s="3">
         <v>86</v>
@@ -5560,7 +5557,7 @@
         <v>6</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F91" s="3">
         <v>87</v>
@@ -5608,7 +5605,7 @@
         <v>24</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F92" s="10">
         <v>90</v>
@@ -5656,7 +5653,7 @@
         <v>45</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F93" s="10">
         <v>92</v>
@@ -5704,7 +5701,7 @@
         <v>6</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F94" s="3">
         <v>92</v>
@@ -5752,7 +5749,7 @@
         <v>55</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F95" s="3">
         <v>92</v>
@@ -5800,7 +5797,7 @@
         <v>57</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F96" s="3">
         <v>92</v>
@@ -5848,7 +5845,7 @@
         <v>188</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F97" s="3">
         <v>100</v>
@@ -5896,7 +5893,7 @@
         <v>28</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F98" s="3">
         <v>102</v>
@@ -5992,7 +5989,7 @@
         <v>187</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F100" s="3">
         <v>123</v>
@@ -6040,7 +6037,7 @@
         <v>6</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F101" s="3">
         <v>124</v>
@@ -6088,7 +6085,7 @@
         <v>45</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F102" s="3">
         <v>126</v>
@@ -6136,7 +6133,7 @@
         <v>6</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F103" s="3">
         <v>126</v>
@@ -6184,7 +6181,7 @@
         <v>23</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F104" s="3">
         <v>132</v>
@@ -6232,7 +6229,7 @@
         <v>6</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F105" s="3">
         <v>135</v>
@@ -6280,7 +6277,7 @@
         <v>187</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F106" s="3">
         <v>151</v>
@@ -6376,7 +6373,7 @@
         <v>24</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F108" s="3">
         <v>165</v>
@@ -6424,7 +6421,7 @@
         <v>6</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F109" s="3">
         <v>180</v>
@@ -6472,7 +6469,7 @@
         <v>6</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F110" s="3">
         <v>180</v>
@@ -6520,7 +6517,7 @@
         <v>182</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F111" s="3">
         <v>182</v>
@@ -6568,7 +6565,7 @@
         <v>32</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F112" s="3">
         <v>204</v>
@@ -6616,7 +6613,7 @@
         <v>6</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F113" s="3">
         <v>210</v>
@@ -6665,7 +6662,7 @@
         <v>6</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F114" s="3">
         <v>215</v>
@@ -6713,7 +6710,7 @@
         <v>22</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F115" s="3">
         <v>228</v>
@@ -6761,7 +6758,7 @@
         <v>186</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F116" s="3">
         <v>233</v>
@@ -6809,7 +6806,7 @@
         <v>22</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F117" s="3">
         <v>241</v>
@@ -6905,7 +6902,7 @@
         <v>46</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F119" s="10">
         <v>256</v>
@@ -6953,7 +6950,7 @@
         <v>186</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F120" s="3">
         <v>256</v>
@@ -7001,7 +6998,7 @@
         <v>45</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F121" s="3">
         <v>257</v>
@@ -7049,7 +7046,7 @@
         <v>38</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F122" s="3">
         <v>261</v>
@@ -7097,7 +7094,7 @@
         <v>55</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F123" s="3">
         <v>268</v>
@@ -7145,7 +7142,7 @@
         <v>180</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F124" s="3">
         <v>316</v>
@@ -7193,7 +7190,7 @@
         <v>38</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F125" s="3">
         <v>322</v>
@@ -7241,7 +7238,7 @@
         <v>45</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F126" s="3">
         <v>324</v>
@@ -7289,7 +7286,7 @@
         <v>6</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F127" s="3">
         <v>338</v>
@@ -7337,7 +7334,7 @@
         <v>46</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F128" s="3">
         <v>344</v>
@@ -7385,7 +7382,7 @@
         <v>24</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F129" s="3">
         <v>347</v>
@@ -7433,7 +7430,7 @@
         <v>6</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F130" s="3">
         <v>370</v>
@@ -7481,7 +7478,7 @@
         <v>32</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F131" s="3">
         <v>387</v>
@@ -7529,7 +7526,7 @@
         <v>41</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F132" s="3">
         <v>395</v>
@@ -7577,7 +7574,7 @@
         <v>6</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F133" s="3">
         <v>400</v>
@@ -7622,7 +7619,7 @@
         <v>185</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F134" s="3">
         <v>435</v>
@@ -7670,7 +7667,7 @@
         <v>182</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F135" s="3">
         <v>458</v>
@@ -7718,7 +7715,7 @@
         <v>22</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F136" s="7">
         <v>466</v>
@@ -7766,7 +7763,7 @@
         <v>52</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F137" s="3">
         <v>483</v>
@@ -7814,7 +7811,7 @@
         <v>32</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F138" s="3">
         <v>493</v>
@@ -7862,7 +7859,7 @@
         <v>6</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F139" s="3">
         <v>530</v>
@@ -7910,7 +7907,7 @@
         <v>51</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F140" s="3">
         <v>530</v>
@@ -7958,7 +7955,7 @@
         <v>185</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F141" s="3">
         <v>537</v>
@@ -8003,7 +8000,7 @@
         <v>6</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F142" s="3">
         <v>570</v>
@@ -8051,7 +8048,7 @@
         <v>45</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F143" s="3">
         <v>590</v>
@@ -8099,7 +8096,7 @@
         <v>41</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F144" s="3">
         <v>671</v>
@@ -8147,7 +8144,7 @@
         <v>36</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F145" s="3">
         <v>690</v>
@@ -8195,7 +8192,7 @@
         <v>20</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F146" s="3">
         <v>702</v>
@@ -8243,7 +8240,7 @@
         <v>28</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F147" s="3">
         <v>733</v>
@@ -8291,7 +8288,7 @@
         <v>182</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F148" s="3">
         <v>735</v>
@@ -8339,7 +8336,7 @@
         <v>29</v>
       </c>
       <c r="E149" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F149" s="7">
         <v>735.3</v>
@@ -8387,7 +8384,7 @@
         <v>38</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F150" s="3">
         <v>749</v>
@@ -8483,7 +8480,7 @@
         <v>180</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F152" s="3">
         <v>784</v>
@@ -8531,7 +8528,7 @@
         <v>6</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F153" s="3">
         <v>879</v>
@@ -8579,7 +8576,7 @@
         <v>37</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F154" s="3">
         <v>887</v>
@@ -8627,7 +8624,7 @@
         <v>36</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F155" s="3">
         <v>917</v>
@@ -8675,7 +8672,7 @@
         <v>50</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F156" s="3">
         <v>950</v>
@@ -8723,7 +8720,7 @@
         <v>36</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F157" s="3">
         <v>979</v>
@@ -8771,7 +8768,7 @@
         <v>180</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F158" s="3">
         <v>988</v>
@@ -8819,7 +8816,7 @@
         <v>6</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F159" s="3">
         <v>1000</v>
@@ -8867,7 +8864,7 @@
         <v>6</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F160" s="3">
         <v>1040</v>
@@ -8915,7 +8912,7 @@
         <v>37</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F161" s="3">
         <v>1044</v>
@@ -8963,7 +8960,7 @@
         <v>24</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F162" s="3">
         <v>1068</v>
@@ -9011,7 +9008,7 @@
         <v>24</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F163" s="3">
         <v>1084</v>
@@ -9059,7 +9056,7 @@
         <v>37</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F164" s="3">
         <v>1091</v>
@@ -9155,7 +9152,7 @@
         <v>28</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F166" s="3">
         <v>1098</v>
@@ -9251,7 +9248,7 @@
         <v>24</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F168" s="3">
         <v>1153</v>
@@ -9299,7 +9296,7 @@
         <v>6</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F169" s="3">
         <v>1200</v>
@@ -9347,7 +9344,7 @@
         <v>41</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F170" s="3">
         <v>1234</v>
@@ -9395,7 +9392,7 @@
         <v>24</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F171" s="3">
         <v>1257</v>
@@ -9443,7 +9440,7 @@
         <v>46</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F172" s="3">
         <v>1400</v>
@@ -9491,7 +9488,7 @@
         <v>20</v>
       </c>
       <c r="E173" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F173" s="3">
         <v>1513</v>
@@ -9536,7 +9533,7 @@
         <v>61</v>
       </c>
       <c r="E174" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F174" s="3">
         <v>1755.6</v>
@@ -9584,7 +9581,7 @@
         <v>28</v>
       </c>
       <c r="E175" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F175" s="3">
         <v>1843</v>
@@ -9632,7 +9629,7 @@
         <v>23</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F176" s="3">
         <v>1875</v>
@@ -9680,7 +9677,7 @@
         <v>6</v>
       </c>
       <c r="E177" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F177" s="3">
         <v>1890</v>
@@ -9728,7 +9725,7 @@
         <v>40</v>
       </c>
       <c r="E178" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F178" s="3">
         <v>1892</v>
@@ -9776,7 +9773,7 @@
         <v>63</v>
       </c>
       <c r="E179" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F179" s="3">
         <v>1971.2</v>
@@ -9872,7 +9869,7 @@
         <v>6</v>
       </c>
       <c r="E181" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F181" s="10">
         <v>2260</v>
@@ -9920,7 +9917,7 @@
         <v>22</v>
       </c>
       <c r="E182" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F182" s="3">
         <v>2382</v>
@@ -9968,7 +9965,7 @@
         <v>64</v>
       </c>
       <c r="E183" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F183" s="3">
         <v>2525.6</v>
@@ -10016,7 +10013,7 @@
         <v>61</v>
       </c>
       <c r="E184" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F184" s="3">
         <v>2872.8</v>
@@ -10064,7 +10061,7 @@
         <v>27</v>
       </c>
       <c r="E185" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F185" s="10">
         <v>2975.4</v>
@@ -10112,7 +10109,7 @@
         <v>40</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F186" s="3">
         <v>2983</v>
@@ -10160,7 +10157,7 @@
         <v>36</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F187" s="3">
         <v>3019</v>
@@ -10208,7 +10205,7 @@
         <v>33</v>
       </c>
       <c r="E188" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F188" s="3">
         <v>3102</v>
@@ -10256,7 +10253,7 @@
         <v>38</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F189" s="3">
         <v>3420</v>
@@ -10304,7 +10301,7 @@
         <v>38</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F190" s="3">
         <v>3624</v>
@@ -10352,7 +10349,7 @@
         <v>37</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F191" s="3">
         <v>3776</v>
@@ -10400,7 +10397,7 @@
         <v>6</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F192" s="3">
         <v>3800</v>
@@ -10448,7 +10445,7 @@
         <v>180</v>
       </c>
       <c r="E193" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F193" s="3">
         <v>3851</v>
@@ -10496,7 +10493,7 @@
         <v>32</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F194" s="3">
         <v>3972</v>
@@ -10508,7 +10505,7 @@
         <v>7</v>
       </c>
       <c r="I194" s="3">
-        <f t="shared" ref="I194:I257" si="12">-LOG(J194)</f>
+        <f t="shared" ref="I194:I253" si="12">-LOG(J194)</f>
         <v>5.7020207558406373</v>
       </c>
       <c r="J194" s="3">
@@ -10544,7 +10541,7 @@
         <v>180</v>
       </c>
       <c r="E195" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F195" s="3">
         <v>4012</v>
@@ -10592,7 +10589,7 @@
         <v>24</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F196" s="3">
         <v>4094</v>
@@ -10640,7 +10637,7 @@
         <v>36</v>
       </c>
       <c r="E197" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F197" s="3">
         <v>4120</v>
@@ -10688,7 +10685,7 @@
         <v>46</v>
       </c>
       <c r="E198" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F198" s="3">
         <v>4500</v>
@@ -10736,7 +10733,7 @@
         <v>46</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F199" s="3">
         <v>4566</v>
@@ -10784,7 +10781,7 @@
         <v>40</v>
       </c>
       <c r="E200" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F200" s="3">
         <v>4604</v>
@@ -10832,7 +10829,7 @@
         <v>28</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F201" s="3">
         <v>4971</v>
@@ -10880,7 +10877,7 @@
         <v>39</v>
       </c>
       <c r="E202" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F202" s="3">
         <v>5658</v>
@@ -10928,7 +10925,7 @@
         <v>32</v>
       </c>
       <c r="E203" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F203" s="3">
         <v>6559</v>
@@ -10976,7 +10973,7 @@
         <v>40</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F204" s="3">
         <v>6836</v>
@@ -11024,7 +11021,7 @@
         <v>32</v>
       </c>
       <c r="E205" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F205" s="3">
         <v>7361</v>
@@ -11072,7 +11069,7 @@
         <v>39</v>
       </c>
       <c r="E206" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F206" s="3">
         <v>7589</v>
@@ -11120,7 +11117,7 @@
         <v>6</v>
       </c>
       <c r="E207" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F207" s="3">
         <v>8300</v>
@@ -11168,7 +11165,7 @@
         <v>41</v>
       </c>
       <c r="E208" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F208" s="3">
         <v>8382</v>
@@ -11216,7 +11213,7 @@
         <v>41</v>
       </c>
       <c r="E209" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F209" s="3">
         <v>9605</v>
@@ -11264,7 +11261,7 @@
         <v>39</v>
       </c>
       <c r="E210" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F210" s="7">
         <v>9834</v>
@@ -11312,7 +11309,7 @@
         <v>180</v>
       </c>
       <c r="E211" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F211" s="3">
         <v>10656</v>
@@ -11360,7 +11357,7 @@
         <v>56</v>
       </c>
       <c r="E212" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F212" s="3">
         <v>10900</v>
@@ -11408,7 +11405,7 @@
         <v>64</v>
       </c>
       <c r="E213" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F213" s="3">
         <v>10961.1</v>
@@ -11456,7 +11453,7 @@
         <v>33</v>
       </c>
       <c r="E214" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F214" s="3">
         <v>14550</v>
@@ -11504,7 +11501,7 @@
         <v>36</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F215" s="3">
         <v>14861</v>
@@ -11552,7 +11549,7 @@
         <v>6</v>
       </c>
       <c r="E216" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F216" s="3">
         <v>15000</v>
@@ -11600,7 +11597,7 @@
         <v>35</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F217" s="3">
         <v>20400</v>
@@ -11648,7 +11645,7 @@
         <v>24</v>
       </c>
       <c r="E218" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F218" s="3">
         <v>20653</v>
@@ -11696,7 +11693,7 @@
         <v>40</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F219" s="3">
         <v>20823</v>
@@ -11744,7 +11741,7 @@
         <v>35</v>
       </c>
       <c r="E220" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F220" s="3">
         <v>22600</v>
@@ -11792,7 +11789,7 @@
         <v>32</v>
       </c>
       <c r="E221" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F221" s="3">
         <v>28750</v>
@@ -11840,7 +11837,7 @@
         <v>6</v>
       </c>
       <c r="E222" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F222" s="3">
         <v>33000</v>
@@ -11888,7 +11885,7 @@
         <v>35</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F223" s="3">
         <v>34200</v>
@@ -11936,7 +11933,7 @@
         <v>33</v>
       </c>
       <c r="E224" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F224" s="3">
         <v>35040</v>
@@ -11984,7 +11981,7 @@
         <v>63</v>
       </c>
       <c r="E225" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F225" s="3">
         <v>41604.300000000003</v>
@@ -12032,7 +12029,7 @@
         <v>40</v>
       </c>
       <c r="E226" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F226" s="3">
         <v>41665</v>
@@ -12080,7 +12077,7 @@
         <v>6</v>
       </c>
       <c r="E227" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F227" s="3">
         <v>43000</v>
@@ -12128,7 +12125,7 @@
         <v>32</v>
       </c>
       <c r="E228" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F228" s="3">
         <v>50000</v>
@@ -12176,7 +12173,7 @@
         <v>32</v>
       </c>
       <c r="E229" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F229" s="3">
         <v>50000</v>
@@ -12224,7 +12221,7 @@
         <v>39</v>
       </c>
       <c r="E230" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F230" s="3">
         <v>50000</v>
@@ -12272,7 +12269,7 @@
         <v>39</v>
       </c>
       <c r="E231" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F231" s="3">
         <v>50000</v>
@@ -12320,7 +12317,7 @@
         <v>39</v>
       </c>
       <c r="E232" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F232" s="3">
         <v>50000</v>
@@ -12368,7 +12365,7 @@
         <v>39</v>
       </c>
       <c r="E233" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F233" s="3">
         <v>50000</v>
@@ -12416,7 +12413,7 @@
         <v>39</v>
       </c>
       <c r="E234" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F234" s="3">
         <v>50000</v>
@@ -12464,7 +12461,7 @@
         <v>55</v>
       </c>
       <c r="E235" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F235" s="3">
         <v>50000</v>
@@ -12512,7 +12509,7 @@
         <v>40</v>
       </c>
       <c r="E236" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F236" s="3">
         <v>50000</v>
@@ -12560,7 +12557,7 @@
         <v>40</v>
       </c>
       <c r="E237" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F237" s="3">
         <v>50000</v>
@@ -12608,7 +12605,7 @@
         <v>37</v>
       </c>
       <c r="E238" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F238" s="3">
         <v>50000</v>
@@ -12656,7 +12653,7 @@
         <v>36</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F239" s="3">
         <v>50000</v>
@@ -12704,7 +12701,7 @@
         <v>36</v>
       </c>
       <c r="E240" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F240" s="3">
         <v>50000</v>
@@ -12800,7 +12797,7 @@
         <v>62</v>
       </c>
       <c r="E242" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F242" s="3">
         <v>50195.6</v>
@@ -12848,7 +12845,7 @@
         <v>26</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F243" s="3">
         <v>77309.100000000006</v>
@@ -12896,7 +12893,7 @@
         <v>27</v>
       </c>
       <c r="E244" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F244" s="10">
         <v>81460.399999999994</v>
@@ -12944,7 +12941,7 @@
         <v>65</v>
       </c>
       <c r="E245" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F245" s="3">
         <v>93979.199999999997</v>
@@ -12992,7 +12989,7 @@
         <v>35</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F246" s="3">
         <v>102600</v>
@@ -13040,7 +13037,7 @@
         <v>29</v>
       </c>
       <c r="E247" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F247" s="10">
         <v>107094.39999999999</v>
@@ -13088,7 +13085,7 @@
         <v>62</v>
       </c>
       <c r="E248" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F248" s="3">
         <v>109645.2</v>
@@ -13136,7 +13133,7 @@
         <v>26</v>
       </c>
       <c r="E249" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F249" s="3">
         <v>110017.60000000001</v>
@@ -13184,7 +13181,7 @@
         <v>65</v>
       </c>
       <c r="E250" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F250" s="3">
         <v>114193.8</v>
@@ -13232,7 +13229,7 @@
         <v>35</v>
       </c>
       <c r="E251" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F251" s="3">
         <v>126800</v>
@@ -13280,7 +13277,7 @@
         <v>33</v>
       </c>
       <c r="E252" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F252" s="3">
         <v>129900</v>
@@ -13328,7 +13325,7 @@
         <v>6</v>
       </c>
       <c r="E253" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F253" s="3">
         <v>257000</v>

</xml_diff>